<commit_message>
simulation with constant etas, import in model
</commit_message>
<xml_diff>
--- a/Data/simul.xlsx
+++ b/Data/simul.xlsx
@@ -534,94 +534,94 @@
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>0.8742605091054259</v>
+        <v>0.9983027155686909</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9133939243465091</v>
+        <v>0.9975444072672697</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9911272648874124</v>
+        <v>0.9967425401755355</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8825514320902368</v>
+        <v>0.9958932501514343</v>
       </c>
       <c r="G2" t="n">
-        <v>0.8969773342235791</v>
+        <v>0.9949922020701396</v>
       </c>
       <c r="H2" t="n">
-        <v>1.016244453622735</v>
+        <v>0.9678462985376345</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9640072201338462</v>
+        <v>0.9643235791144832</v>
       </c>
       <c r="J2" t="n">
-        <v>1.002542980363822</v>
+        <v>0.9603420500063534</v>
       </c>
       <c r="K2" t="n">
-        <v>1.067875520141275</v>
+        <v>0.9558058322794803</v>
       </c>
       <c r="L2" t="n">
-        <v>0.8710479177817908</v>
+        <v>0.9505903319352602</v>
       </c>
       <c r="M2" t="n">
-        <v>0.8834171382167233</v>
+        <v>0.9642821975634905</v>
       </c>
       <c r="N2" t="n">
-        <v>0.8577839981684531</v>
+        <v>0.9602951012356563</v>
       </c>
       <c r="O2" t="n">
-        <v>0.8734621113500713</v>
+        <v>0.9557521123158824</v>
       </c>
       <c r="P2" t="n">
-        <v>0.8839206142198985</v>
+        <v>0.9505282628582306</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.8758797485667907</v>
+        <v>0.9444580925643837</v>
       </c>
       <c r="R2" t="n">
-        <v>0.8808897156945679</v>
+        <v>0.9399321550946919</v>
       </c>
       <c r="S2" t="n">
-        <v>0.8523642856454163</v>
+        <v>0.9319322926485022</v>
       </c>
       <c r="T2" t="n">
-        <v>0.9060380465680608</v>
+        <v>0.9222815462117561</v>
       </c>
       <c r="U2" t="n">
-        <v>0.871146206663179</v>
+        <v>0.9104100959706604</v>
       </c>
       <c r="V2" t="n">
-        <v>0.8714819148913966</v>
+        <v>0.8954517889565159</v>
       </c>
       <c r="W2" t="n">
-        <v>0.8055862822495766</v>
+        <v>0.8772976549101796</v>
       </c>
       <c r="X2" t="n">
-        <v>0.9587261707961964</v>
+        <v>0.851526041981217</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.8265321616957053</v>
+        <v>0.8149013742522324</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.6858370084810015</v>
+        <v>0.7587393334643031</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.6529712039268099</v>
+        <v>0.6617201467588985</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.3921115269125077</v>
+        <v>0.4515476998849652</v>
       </c>
       <c r="AC2" t="n">
-        <v>-0.442563741422304</v>
+        <v>-0.3214907739752885</v>
       </c>
       <c r="AD2" t="n">
-        <v>-4.881016813889054</v>
+        <v>-4.856760037084229</v>
       </c>
       <c r="AE2" t="n">
-        <v>-1.825660326528651</v>
+        <v>-1.769711727294768</v>
       </c>
       <c r="AF2" t="n">
-        <v>-1.40427077085056</v>
+        <v>-1.417487766727071</v>
       </c>
     </row>
     <row r="3">
@@ -630,94 +630,94 @@
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
-        <v>0.8904115846379687</v>
+        <v>0.9555826385044416</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9581909300060394</v>
+        <v>0.9548243302030204</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9645155457953256</v>
+        <v>0.9540224631112862</v>
       </c>
       <c r="F3" t="n">
-        <v>1.025283588629158</v>
+        <v>0.953173173087185</v>
       </c>
       <c r="G3" t="n">
-        <v>1.07596889772565</v>
+        <v>0.9522721250058903</v>
       </c>
       <c r="H3" t="n">
-        <v>1.036129897043996</v>
+        <v>0.9251262214733852</v>
       </c>
       <c r="I3" t="n">
-        <v>1.002904862511704</v>
+        <v>0.9216035020502339</v>
       </c>
       <c r="J3" t="n">
-        <v>0.8912515254544469</v>
+        <v>0.9176219729421041</v>
       </c>
       <c r="K3" t="n">
-        <v>0.8476228010133016</v>
+        <v>0.9130857552152311</v>
       </c>
       <c r="L3" t="n">
-        <v>1.093814075146556</v>
+        <v>0.9078702548710109</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8907961552306536</v>
+        <v>0.9215621204992412</v>
       </c>
       <c r="N3" t="n">
-        <v>0.98458051585041</v>
+        <v>0.917575024171407</v>
       </c>
       <c r="O3" t="n">
-        <v>0.883221242891432</v>
+        <v>0.9130320352516331</v>
       </c>
       <c r="P3" t="n">
-        <v>0.830578770985769</v>
+        <v>0.9078081857939813</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.8998542524983211</v>
+        <v>0.9017380155001344</v>
       </c>
       <c r="R3" t="n">
-        <v>0.8466370798188856</v>
+        <v>0.8972120780304426</v>
       </c>
       <c r="S3" t="n">
-        <v>0.8300338630711219</v>
+        <v>0.8892122155842529</v>
       </c>
       <c r="T3" t="n">
-        <v>0.9074246528209691</v>
+        <v>0.8795614691475068</v>
       </c>
       <c r="U3" t="n">
-        <v>0.882843152199872</v>
+        <v>0.8676900189064111</v>
       </c>
       <c r="V3" t="n">
-        <v>1.003546224805913</v>
+        <v>0.8527317118922666</v>
       </c>
       <c r="W3" t="n">
-        <v>0.771476336107738</v>
+        <v>0.8345775778459303</v>
       </c>
       <c r="X3" t="n">
-        <v>0.8897583433868615</v>
+        <v>0.8088059649169677</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.7289208547449677</v>
+        <v>0.7721812971879831</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.9950073780099683</v>
+        <v>0.7160192564000538</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.5664510910983831</v>
+        <v>0.6190000696946492</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.486803571700862</v>
+        <v>0.408827622820716</v>
       </c>
       <c r="AC3" t="n">
-        <v>-0.4375044273770408</v>
+        <v>-0.3642108510395377</v>
       </c>
       <c r="AD3" t="n">
-        <v>-4.880985181098043</v>
+        <v>-4.899480114148478</v>
       </c>
       <c r="AE3" t="n">
-        <v>-1.755359363949666</v>
+        <v>-1.812431804359017</v>
       </c>
       <c r="AF3" t="n">
-        <v>-1.537822098838399</v>
+        <v>-1.46020784379132</v>
       </c>
     </row>
     <row r="4">
@@ -726,94 +726,94 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
-        <v>0.9059853961069145</v>
+        <v>0.9596781156805632</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8919832791386524</v>
+        <v>0.9589198073791421</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9901447296864835</v>
+        <v>0.9581179402874078</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8717250249797104</v>
+        <v>0.9572686502633065</v>
       </c>
       <c r="G4" t="n">
-        <v>1.1148826965075</v>
+        <v>0.956367602182012</v>
       </c>
       <c r="H4" t="n">
-        <v>0.8465423614581538</v>
+        <v>0.9292216986495068</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9197551377805405</v>
+        <v>0.9256989792263555</v>
       </c>
       <c r="J4" t="n">
-        <v>0.8387459233192111</v>
+        <v>0.9217174501182257</v>
       </c>
       <c r="K4" t="n">
-        <v>0.868466102597391</v>
+        <v>0.9171812323913526</v>
       </c>
       <c r="L4" t="n">
-        <v>1.009714880584353</v>
+        <v>0.9119657320471326</v>
       </c>
       <c r="M4" t="n">
-        <v>0.9186562917212305</v>
+        <v>0.9256575976753629</v>
       </c>
       <c r="N4" t="n">
-        <v>1.015567359773934</v>
+        <v>0.9216705013475286</v>
       </c>
       <c r="O4" t="n">
-        <v>0.8927233071378969</v>
+        <v>0.9171275124277547</v>
       </c>
       <c r="P4" t="n">
-        <v>1.120056341267199</v>
+        <v>0.9119036629701029</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.8328154660407485</v>
+        <v>0.9058334926762561</v>
       </c>
       <c r="R4" t="n">
-        <v>0.9111380262492217</v>
+        <v>0.9013075552065641</v>
       </c>
       <c r="S4" t="n">
-        <v>0.8493708750863567</v>
+        <v>0.8933076927603745</v>
       </c>
       <c r="T4" t="n">
-        <v>0.826588462441925</v>
+        <v>0.8836569463236283</v>
       </c>
       <c r="U4" t="n">
-        <v>0.877402602195265</v>
+        <v>0.8717854960825326</v>
       </c>
       <c r="V4" t="n">
-        <v>0.8897719849325137</v>
+        <v>0.8568271890683883</v>
       </c>
       <c r="W4" t="n">
-        <v>0.8651630532832451</v>
+        <v>0.838673055022052</v>
       </c>
       <c r="X4" t="n">
-        <v>0.7734412443197245</v>
+        <v>0.8129014420930893</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.9532107205649918</v>
+        <v>0.7762767743641048</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.6441245868769263</v>
+        <v>0.7201147335761755</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.5456842776202364</v>
+        <v>0.6230955468707708</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.4246375206622264</v>
+        <v>0.4129230999968376</v>
       </c>
       <c r="AC4" t="n">
-        <v>-0.402626821456376</v>
+        <v>-0.3601153738634161</v>
       </c>
       <c r="AD4" t="n">
-        <v>-4.955589633941067</v>
+        <v>-4.895384636972357</v>
       </c>
       <c r="AE4" t="n">
-        <v>-1.860001444164148</v>
+        <v>-1.808336327182895</v>
       </c>
       <c r="AF4" t="n">
-        <v>-1.450482499328467</v>
+        <v>-1.456112366615198</v>
       </c>
     </row>
     <row r="5">
@@ -822,94 +822,94 @@
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="n">
-        <v>0.9853295627453388</v>
+        <v>1.095161147701316</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9199074504551277</v>
+        <v>1.094402839399894</v>
       </c>
       <c r="E5" t="n">
-        <v>1.10608988847742</v>
+        <v>1.09360097230816</v>
       </c>
       <c r="F5" t="n">
-        <v>0.8824507926181812</v>
+        <v>1.092751682284059</v>
       </c>
       <c r="G5" t="n">
-        <v>0.90928981499798</v>
+        <v>1.091850634202764</v>
       </c>
       <c r="H5" t="n">
-        <v>0.8704992891182032</v>
+        <v>1.064704730670259</v>
       </c>
       <c r="I5" t="n">
-        <v>1.099234461962014</v>
+        <v>1.061182011247108</v>
       </c>
       <c r="J5" t="n">
-        <v>1.043875609254461</v>
+        <v>1.057200482138978</v>
       </c>
       <c r="K5" t="n">
-        <v>0.8382636434740722</v>
+        <v>1.052664264412105</v>
       </c>
       <c r="L5" t="n">
-        <v>0.8368707033823104</v>
+        <v>1.047448764067885</v>
       </c>
       <c r="M5" t="n">
-        <v>0.8907001320491776</v>
+        <v>1.061140629696115</v>
       </c>
       <c r="N5" t="n">
-        <v>1.066173952647927</v>
+        <v>1.057153533368281</v>
       </c>
       <c r="O5" t="n">
-        <v>0.8607438094807138</v>
+        <v>1.052610544448507</v>
       </c>
       <c r="P5" t="n">
-        <v>1.089902962503898</v>
+        <v>1.047386694990855</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.8862484280363092</v>
+        <v>1.041316524697008</v>
       </c>
       <c r="R5" t="n">
-        <v>1.050259344242794</v>
+        <v>1.036790587227316</v>
       </c>
       <c r="S5" t="n">
-        <v>1.033703116870835</v>
+        <v>1.028790724781127</v>
       </c>
       <c r="T5" t="n">
-        <v>1.008976626561611</v>
+        <v>1.019139978344381</v>
       </c>
       <c r="U5" t="n">
-        <v>0.9562941277886929</v>
+        <v>1.007268528103285</v>
       </c>
       <c r="V5" t="n">
-        <v>0.9382807175465535</v>
+        <v>0.9923102210891406</v>
       </c>
       <c r="W5" t="n">
-        <v>0.8463592215243745</v>
+        <v>0.9741560870428043</v>
       </c>
       <c r="X5" t="n">
-        <v>0.7798503607031279</v>
+        <v>0.9483844741138416</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.868199858379086</v>
+        <v>0.9117598063848571</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.6601049034156907</v>
+        <v>0.8555977655969278</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.6495814401442181</v>
+        <v>0.7585785788915231</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.5767680896049817</v>
+        <v>0.5484061320175899</v>
       </c>
       <c r="AC5" t="n">
-        <v>-0.2176917350394171</v>
+        <v>-0.2246323418426638</v>
       </c>
       <c r="AD5" t="n">
-        <v>-4.892083956361225</v>
+        <v>-4.759901604951605</v>
       </c>
       <c r="AE5" t="n">
-        <v>-1.84810106792664</v>
+        <v>-1.672853295162143</v>
       </c>
       <c r="AF5" t="n">
-        <v>-1.408610476205393</v>
+        <v>-1.320629334594446</v>
       </c>
     </row>
     <row r="6">
@@ -918,94 +918,94 @@
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
-        <v>0.9833284705332145</v>
+        <v>0.9223288234291217</v>
       </c>
       <c r="D6" t="n">
-        <v>1.021967477812755</v>
+        <v>0.9215705151277005</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9607162846488142</v>
+        <v>0.9207686480359664</v>
       </c>
       <c r="F6" t="n">
-        <v>1.255562739211629</v>
+        <v>0.9199193580118651</v>
       </c>
       <c r="G6" t="n">
-        <v>0.8793552396710973</v>
+        <v>0.9190183099305704</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9872831838061495</v>
+        <v>0.8918724063980653</v>
       </c>
       <c r="I6" t="n">
-        <v>0.8543464414696575</v>
+        <v>0.888349686974914</v>
       </c>
       <c r="J6" t="n">
-        <v>1.022331261188735</v>
+        <v>0.8843681578667842</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8435929821254305</v>
+        <v>0.8798319401399112</v>
       </c>
       <c r="L6" t="n">
-        <v>0.9138924181169763</v>
+        <v>0.874616439795691</v>
       </c>
       <c r="M6" t="n">
-        <v>0.9142052156809712</v>
+        <v>0.8883083054239214</v>
       </c>
       <c r="N6" t="n">
-        <v>0.8477564886001783</v>
+        <v>0.8843212090960871</v>
       </c>
       <c r="O6" t="n">
-        <v>0.853294656047933</v>
+        <v>0.8797782201763132</v>
       </c>
       <c r="P6" t="n">
-        <v>0.826504460887011</v>
+        <v>0.8745543707186614</v>
       </c>
       <c r="Q6" t="n">
-        <v>1.080418059409393</v>
+        <v>0.8684842004248146</v>
       </c>
       <c r="R6" t="n">
-        <v>1.196560249113378</v>
+        <v>0.8639582629551227</v>
       </c>
       <c r="S6" t="n">
-        <v>0.8645551008241794</v>
+        <v>0.855958400508933</v>
       </c>
       <c r="T6" t="n">
-        <v>0.9827261748784153</v>
+        <v>0.8463076540721869</v>
       </c>
       <c r="U6" t="n">
-        <v>0.7850611792360813</v>
+        <v>0.8344362038310912</v>
       </c>
       <c r="V6" t="n">
-        <v>0.7776233190511769</v>
+        <v>0.8194778968169467</v>
       </c>
       <c r="W6" t="n">
-        <v>1.125370070868396</v>
+        <v>0.8013237627706105</v>
       </c>
       <c r="X6" t="n">
-        <v>0.7485800039969652</v>
+        <v>0.7755521498416478</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.8849294371615068</v>
+        <v>0.7389274821126632</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.7558764707135868</v>
+        <v>0.6827654413247339</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.728696731095549</v>
+        <v>0.5857462546193293</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.374507393312817</v>
+        <v>0.3755738077453961</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.0170209136578976</v>
+        <v>-0.3974646661148576</v>
       </c>
       <c r="AD6" t="n">
-        <v>-4.741215217023163</v>
+        <v>-4.932733929223798</v>
       </c>
       <c r="AE6" t="n">
-        <v>-1.864082788917866</v>
+        <v>-1.845685619434337</v>
       </c>
       <c r="AF6" t="n">
-        <v>-1.306828628502802</v>
+        <v>-1.49346165886664</v>
       </c>
     </row>
     <row r="7">
@@ -1014,94 +1014,94 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
-        <v>0.9620395663637522</v>
+        <v>0.9767056701777337</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9338945795872569</v>
+        <v>0.9759473618763125</v>
       </c>
       <c r="E7" t="n">
-        <v>0.8996118061296371</v>
+        <v>0.9751454947845783</v>
       </c>
       <c r="F7" t="n">
-        <v>1.021505525869682</v>
+        <v>0.9742962047604771</v>
       </c>
       <c r="G7" t="n">
-        <v>0.8906816397151129</v>
+        <v>0.9733951566791824</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8524524270224353</v>
+        <v>0.9462492531466773</v>
       </c>
       <c r="I7" t="n">
-        <v>1.017834818772043</v>
+        <v>0.942726533723526</v>
       </c>
       <c r="J7" t="n">
-        <v>0.8812481590522274</v>
+        <v>0.9387450046153962</v>
       </c>
       <c r="K7" t="n">
-        <v>0.8386278385464415</v>
+        <v>0.9342087868885232</v>
       </c>
       <c r="L7" t="n">
-        <v>0.9208882194923889</v>
+        <v>0.928993286544303</v>
       </c>
       <c r="M7" t="n">
-        <v>0.9928380588341188</v>
+        <v>0.9426851521725333</v>
       </c>
       <c r="N7" t="n">
-        <v>1.002770365880311</v>
+        <v>0.9386980558446991</v>
       </c>
       <c r="O7" t="n">
-        <v>1.070266513065699</v>
+        <v>0.9341550669249252</v>
       </c>
       <c r="P7" t="n">
-        <v>0.9444389597441979</v>
+        <v>0.9289312174672734</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.8754580506283811</v>
+        <v>0.9228610471734265</v>
       </c>
       <c r="R7" t="n">
-        <v>0.8345513624012491</v>
+        <v>0.9183351097037347</v>
       </c>
       <c r="S7" t="n">
-        <v>0.9535862281655076</v>
+        <v>0.910335247257545</v>
       </c>
       <c r="T7" t="n">
-        <v>0.9144798833024297</v>
+        <v>0.9006845008207989</v>
       </c>
       <c r="U7" t="n">
-        <v>0.823475998775631</v>
+        <v>0.8888130505797032</v>
       </c>
       <c r="V7" t="n">
-        <v>0.7760589316701296</v>
+        <v>0.8738547435655587</v>
       </c>
       <c r="W7" t="n">
-        <v>0.9687370374027371</v>
+        <v>0.8557006095192224</v>
       </c>
       <c r="X7" t="n">
-        <v>0.9269043266125835</v>
+        <v>0.8299289965902598</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.7655127544873671</v>
+        <v>0.7933043288612752</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.755260457121895</v>
+        <v>0.7371422880733459</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.5551383827461044</v>
+        <v>0.6401231013679413</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.3721041366182585</v>
+        <v>0.429950654494008</v>
       </c>
       <c r="AC7" t="n">
-        <v>-0.4063165983033654</v>
+        <v>-0.3430878193662457</v>
       </c>
       <c r="AD7" t="n">
-        <v>-4.972740432082962</v>
+        <v>-4.878357082475186</v>
       </c>
       <c r="AE7" t="n">
-        <v>-1.821081134707227</v>
+        <v>-1.791308772685725</v>
       </c>
       <c r="AF7" t="n">
-        <v>-1.435629440144831</v>
+        <v>-1.439084812118028</v>
       </c>
     </row>
     <row r="8">
@@ -1110,94 +1110,94 @@
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
-        <v>1.094177108654658</v>
+        <v>0.8965646696254003</v>
       </c>
       <c r="D8" t="n">
-        <v>1.05061340770323</v>
+        <v>0.8958063613239791</v>
       </c>
       <c r="E8" t="n">
-        <v>0.973833622987387</v>
+        <v>0.8950044942322449</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9652405382600203</v>
+        <v>0.8941552042081437</v>
       </c>
       <c r="G8" t="n">
-        <v>0.9849537926037711</v>
+        <v>0.893254156126849</v>
       </c>
       <c r="H8" t="n">
-        <v>0.88583383973776</v>
+        <v>0.8661082525943439</v>
       </c>
       <c r="I8" t="n">
-        <v>0.9135112970055959</v>
+        <v>0.8625855331711926</v>
       </c>
       <c r="J8" t="n">
-        <v>0.9710160726568966</v>
+        <v>0.8586040040630628</v>
       </c>
       <c r="K8" t="n">
-        <v>1.038141632893465</v>
+        <v>0.8540677863361897</v>
       </c>
       <c r="L8" t="n">
-        <v>0.9404812441048156</v>
+        <v>0.8488522859919696</v>
       </c>
       <c r="M8" t="n">
-        <v>0.9695552779467299</v>
+        <v>0.8625441516201999</v>
       </c>
       <c r="N8" t="n">
-        <v>0.8701771776063619</v>
+        <v>0.8585570552923657</v>
       </c>
       <c r="O8" t="n">
-        <v>0.8993184255042163</v>
+        <v>0.8540140663725918</v>
       </c>
       <c r="P8" t="n">
-        <v>0.8533242012845992</v>
+        <v>0.8487902169149399</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.8657782884303468</v>
+        <v>0.8427200466210931</v>
       </c>
       <c r="R8" t="n">
-        <v>0.8222035728216337</v>
+        <v>0.8381941091514012</v>
       </c>
       <c r="S8" t="n">
-        <v>0.8287084753082732</v>
+        <v>0.8301942467052116</v>
       </c>
       <c r="T8" t="n">
-        <v>0.8597256698945046</v>
+        <v>0.8205435002684655</v>
       </c>
       <c r="U8" t="n">
-        <v>1.055291713760738</v>
+        <v>0.8086720500273697</v>
       </c>
       <c r="V8" t="n">
-        <v>0.9478328427059486</v>
+        <v>0.7937137430132253</v>
       </c>
       <c r="W8" t="n">
-        <v>0.8117039402646981</v>
+        <v>0.775559608966889</v>
       </c>
       <c r="X8" t="n">
-        <v>0.816276703488355</v>
+        <v>0.7497879960379263</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.7852511639601667</v>
+        <v>0.7131633283089418</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.6711603902405809</v>
+        <v>0.6570012875210125</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.7328484890139747</v>
+        <v>0.5599821008156078</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.4886021732027125</v>
+        <v>0.3498096539416746</v>
       </c>
       <c r="AC8" t="n">
-        <v>-0.3851403911021362</v>
+        <v>-0.4232288199185791</v>
       </c>
       <c r="AD8" t="n">
-        <v>-4.968744097921314</v>
+        <v>-4.95849808302752</v>
       </c>
       <c r="AE8" t="n">
-        <v>-1.722580113629792</v>
+        <v>-1.871449773238058</v>
       </c>
       <c r="AF8" t="n">
-        <v>-1.538197185431717</v>
+        <v>-1.519225812670361</v>
       </c>
     </row>
     <row r="9">
@@ -1206,94 +1206,94 @@
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="n">
-        <v>1.000583411282661</v>
+        <v>0.9595701115408425</v>
       </c>
       <c r="D9" t="n">
-        <v>1.196914232713509</v>
+        <v>0.9588118032394213</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9866732072802614</v>
+        <v>0.9580099361476871</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9994043663520744</v>
+        <v>0.9571606461235859</v>
       </c>
       <c r="G9" t="n">
-        <v>0.9602706193351792</v>
+        <v>0.9562595980422912</v>
       </c>
       <c r="H9" t="n">
-        <v>1.016657127741021</v>
+        <v>0.9291136945097861</v>
       </c>
       <c r="I9" t="n">
-        <v>0.8446311992021713</v>
+        <v>0.9255909750866348</v>
       </c>
       <c r="J9" t="n">
-        <v>0.8835657158847795</v>
+        <v>0.921609445978505</v>
       </c>
       <c r="K9" t="n">
-        <v>0.8591852189840776</v>
+        <v>0.917073228251632</v>
       </c>
       <c r="L9" t="n">
-        <v>0.8300402721834093</v>
+        <v>0.9118577279074118</v>
       </c>
       <c r="M9" t="n">
-        <v>0.9012128072277142</v>
+        <v>0.9255495935356421</v>
       </c>
       <c r="N9" t="n">
-        <v>0.9507848895179717</v>
+        <v>0.9215624972078079</v>
       </c>
       <c r="O9" t="n">
-        <v>1.17788877300291</v>
+        <v>0.917019508288034</v>
       </c>
       <c r="P9" t="n">
-        <v>1.012334151577501</v>
+        <v>0.9117956588303822</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.9533851347306491</v>
+        <v>0.9057254885365353</v>
       </c>
       <c r="R9" t="n">
-        <v>0.8337523162945902</v>
+        <v>0.9011995510668435</v>
       </c>
       <c r="S9" t="n">
-        <v>0.8963401425235705</v>
+        <v>0.8931996886206538</v>
       </c>
       <c r="T9" t="n">
-        <v>0.874315634922862</v>
+        <v>0.8835489421839077</v>
       </c>
       <c r="U9" t="n">
-        <v>0.9157949212092481</v>
+        <v>0.871677491942812</v>
       </c>
       <c r="V9" t="n">
-        <v>0.8241099281213953</v>
+        <v>0.8567191849286675</v>
       </c>
       <c r="W9" t="n">
-        <v>0.7746659824862999</v>
+        <v>0.8385650508823312</v>
       </c>
       <c r="X9" t="n">
-        <v>0.9000908670898753</v>
+        <v>0.8127934379533686</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.6896740042911267</v>
+        <v>0.776168770224384</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.7984997078123088</v>
+        <v>0.7200067294364547</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.5710224198408893</v>
+        <v>0.6229875427310501</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.3953064650824751</v>
+        <v>0.4128150958571168</v>
       </c>
       <c r="AC9" t="n">
-        <v>-0.4326461958702888</v>
+        <v>-0.3602233780031369</v>
       </c>
       <c r="AD9" t="n">
-        <v>-4.881482931589568</v>
+        <v>-4.895492641112077</v>
       </c>
       <c r="AE9" t="n">
-        <v>-1.817975994991557</v>
+        <v>-1.808444331322616</v>
       </c>
       <c r="AF9" t="n">
-        <v>-1.402434298532479</v>
+        <v>-1.456220370754919</v>
       </c>
     </row>
     <row r="10">
@@ -1302,94 +1302,94 @@
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="n">
-        <v>1.007267623935857</v>
+        <v>1.01731163995365</v>
       </c>
       <c r="D10" t="n">
-        <v>0.9306043139771542</v>
+        <v>1.016553331652229</v>
       </c>
       <c r="E10" t="n">
-        <v>0.9179709660869283</v>
+        <v>1.015751464560495</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9157454327891873</v>
+        <v>1.014902174536393</v>
       </c>
       <c r="G10" t="n">
-        <v>1.105406466321655</v>
+        <v>1.014001126455099</v>
       </c>
       <c r="H10" t="n">
-        <v>1.059132126574475</v>
+        <v>0.9868552229225935</v>
       </c>
       <c r="I10" t="n">
-        <v>0.9159119765987008</v>
+        <v>0.9833325034994422</v>
       </c>
       <c r="J10" t="n">
-        <v>0.8657465069164585</v>
+        <v>0.9793509743913125</v>
       </c>
       <c r="K10" t="n">
-        <v>0.9581242883583552</v>
+        <v>0.9748147566644394</v>
       </c>
       <c r="L10" t="n">
-        <v>0.948369316792669</v>
+        <v>0.9695992563202191</v>
       </c>
       <c r="M10" t="n">
-        <v>0.9607489138813544</v>
+        <v>0.9832911219484495</v>
       </c>
       <c r="N10" t="n">
-        <v>0.857316340673918</v>
+        <v>0.9793040256206154</v>
       </c>
       <c r="O10" t="n">
-        <v>0.8675546096697135</v>
+        <v>0.9747610367008415</v>
       </c>
       <c r="P10" t="n">
-        <v>0.8621435771601909</v>
+        <v>0.9695371872431895</v>
       </c>
       <c r="Q10" t="n">
-        <v>1.075959281562803</v>
+        <v>0.9634670169493427</v>
       </c>
       <c r="R10" t="n">
-        <v>0.8892289267060213</v>
+        <v>0.9589410794796509</v>
       </c>
       <c r="S10" t="n">
-        <v>1.141151497449762</v>
+        <v>0.9509412170334612</v>
       </c>
       <c r="T10" t="n">
-        <v>0.8170195355530449</v>
+        <v>0.9412904705967151</v>
       </c>
       <c r="U10" t="n">
-        <v>0.8305591866949271</v>
+        <v>0.9294190203556194</v>
       </c>
       <c r="V10" t="n">
-        <v>0.8183655798864214</v>
+        <v>0.9144607133414748</v>
       </c>
       <c r="W10" t="n">
-        <v>0.7840471431055368</v>
+        <v>0.8963065792951386</v>
       </c>
       <c r="X10" t="n">
-        <v>0.7315786003656926</v>
+        <v>0.8705349663661759</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.6909333215933439</v>
+        <v>0.8339102986371913</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.7209928756319314</v>
+        <v>0.777748257849262</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.6676373487973384</v>
+        <v>0.6807290711438574</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.3265542501975831</v>
+        <v>0.4705566242699242</v>
       </c>
       <c r="AC10" t="n">
-        <v>-0.3397916371324881</v>
+        <v>-0.3024818495903295</v>
       </c>
       <c r="AD10" t="n">
-        <v>-4.847557134205025</v>
+        <v>-4.837751112699269</v>
       </c>
       <c r="AE10" t="n">
-        <v>-1.618333272875404</v>
+        <v>-1.750702802909809</v>
       </c>
       <c r="AF10" t="n">
-        <v>-1.427190802972579</v>
+        <v>-1.398478842342112</v>
       </c>
     </row>
     <row r="11">
@@ -1398,94 +1398,94 @@
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="n">
-        <v>1.025008224755171</v>
+        <v>0.9471859259392015</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9033387793665144</v>
+        <v>0.9464276176377803</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9221063882097377</v>
+        <v>0.9456257505460461</v>
       </c>
       <c r="F11" t="n">
-        <v>0.8848273631485157</v>
+        <v>0.9447764605219449</v>
       </c>
       <c r="G11" t="n">
-        <v>0.877499822033924</v>
+        <v>0.9438754124406502</v>
       </c>
       <c r="H11" t="n">
-        <v>0.8530525816854675</v>
+        <v>0.9167295089081451</v>
       </c>
       <c r="I11" t="n">
-        <v>0.85646267814261</v>
+        <v>0.9132067894849938</v>
       </c>
       <c r="J11" t="n">
-        <v>0.948461048406549</v>
+        <v>0.909225260376864</v>
       </c>
       <c r="K11" t="n">
-        <v>1.143522597095046</v>
+        <v>0.9046890426499909</v>
       </c>
       <c r="L11" t="n">
-        <v>0.8861485742013846</v>
+        <v>0.8994735423057708</v>
       </c>
       <c r="M11" t="n">
-        <v>1.066056287280284</v>
+        <v>0.9131654079340011</v>
       </c>
       <c r="N11" t="n">
-        <v>0.8954042260711492</v>
+        <v>0.9091783116061669</v>
       </c>
       <c r="O11" t="n">
-        <v>0.9244119774422903</v>
+        <v>0.904635322686393</v>
       </c>
       <c r="P11" t="n">
-        <v>0.8274428913860927</v>
+        <v>0.8994114732287412</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.844148518174147</v>
+        <v>0.8933413029348943</v>
       </c>
       <c r="R11" t="n">
-        <v>0.8794652600386295</v>
+        <v>0.8888153654652025</v>
       </c>
       <c r="S11" t="n">
-        <v>0.8148736439740505</v>
+        <v>0.8808155030190128</v>
       </c>
       <c r="T11" t="n">
-        <v>0.8708850776077905</v>
+        <v>0.8711647565822667</v>
       </c>
       <c r="U11" t="n">
-        <v>0.851596173617021</v>
+        <v>0.859293306341171</v>
       </c>
       <c r="V11" t="n">
-        <v>0.8528107483877624</v>
+        <v>0.8443349993270265</v>
       </c>
       <c r="W11" t="n">
-        <v>0.7652317842432466</v>
+        <v>0.8261808652806902</v>
       </c>
       <c r="X11" t="n">
-        <v>0.7354181014868396</v>
+        <v>0.8004092523517276</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.7012137680781139</v>
+        <v>0.763784584622743</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.6458938587731937</v>
+        <v>0.7076225438348137</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.6925343857395332</v>
+        <v>0.6106033571294091</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.4234461739892804</v>
+        <v>0.4004309102554758</v>
       </c>
       <c r="AC11" t="n">
-        <v>-0.4222828032733138</v>
+        <v>-0.3726075636047779</v>
       </c>
       <c r="AD11" t="n">
-        <v>-4.800820670296815</v>
+        <v>-4.907876826713718</v>
       </c>
       <c r="AE11" t="n">
-        <v>-1.818577462822673</v>
+        <v>-1.820828516924257</v>
       </c>
       <c r="AF11" t="n">
-        <v>-1.518047164029428</v>
+        <v>-1.46860455635656</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
simulation with two scenarios, corrected time shift, probas correctly detect Net Zero and CurPo
</commit_message>
<xml_diff>
--- a/Data/simul.xlsx
+++ b/Data/simul.xlsx
@@ -2,28 +2,33 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Net Zero 2050" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Current Policies" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <sz val="11"/>
     </font>
     <font>
       <b val="1"/>
@@ -37,12 +42,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -55,16 +75,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -147,44 +170,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -211,14 +234,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -245,6 +269,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -256,170 +281,1210 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AF11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="n">
+        <v>2020</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>2023</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>2024</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>2025</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>2026</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>2027</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>2028</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>2029</v>
+      </c>
+      <c r="L1" s="1" t="n">
+        <v>2030</v>
+      </c>
+      <c r="M1" s="1" t="n">
+        <v>2031</v>
+      </c>
+      <c r="N1" s="1" t="n">
+        <v>2032</v>
+      </c>
+      <c r="O1" s="1" t="n">
+        <v>2033</v>
+      </c>
+      <c r="P1" s="1" t="n">
+        <v>2034</v>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>2035</v>
+      </c>
+      <c r="R1" s="1" t="n">
+        <v>2036</v>
+      </c>
+      <c r="S1" s="1" t="n">
+        <v>2037</v>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>2038</v>
+      </c>
+      <c r="U1" s="1" t="n">
+        <v>2039</v>
+      </c>
+      <c r="V1" s="1" t="n">
+        <v>2040</v>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>2041</v>
+      </c>
+      <c r="X1" s="1" t="n">
+        <v>2042</v>
+      </c>
+      <c r="Y1" s="1" t="n">
+        <v>2043</v>
+      </c>
+      <c r="Z1" s="1" t="n">
+        <v>2044</v>
+      </c>
+      <c r="AA1" s="1" t="n">
+        <v>2045</v>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>2046</v>
+      </c>
+      <c r="AC1" s="1" t="n">
+        <v>2047</v>
+      </c>
+      <c r="AD1" s="1" t="n">
+        <v>2048</v>
+      </c>
+      <c r="AE1" s="1" t="n">
+        <v>2049</v>
+      </c>
+      <c r="AF1" s="1" t="n">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9278600125510837</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9271017042496625</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.9262998371579284</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9254505471338271</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.9245494990525325</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.8974035955200274</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.8938808760968761</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.8898993469887463</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.8853631292618732</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.8801476289176531</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.8938394945458834</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.8898523982180492</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.8853094092982753</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.8800855598406234</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.8740153895467766</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.8694894520770847</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.8614895896308951</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.8518388431941489</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.8399673929530532</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.8250090859389088</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.8068549518925725</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.7810833389636098</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.7444586712346253</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.688296630446696</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.5912774437412913</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.381104996867358</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>-0.3919334769928957</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>-4.927202740101836</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>-1.840154430312375</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>-1.487930469744678</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.124451722829558</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.123693414528137</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.122891547436403</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.122042257412301</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1.121141209331007</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1.093995305798502</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1.09047258637535</v>
+      </c>
+      <c r="J3" t="n">
+        <v>1.086491057267221</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1.081954839540348</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1.076739339196127</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1.090431204824358</v>
+      </c>
+      <c r="N3" t="n">
+        <v>1.086444108496524</v>
+      </c>
+      <c r="O3" t="n">
+        <v>1.08190111957675</v>
+      </c>
+      <c r="P3" t="n">
+        <v>1.076677270119098</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>1.070607099825251</v>
+      </c>
+      <c r="R3" t="n">
+        <v>1.066081162355559</v>
+      </c>
+      <c r="S3" t="n">
+        <v>1.058081299909369</v>
+      </c>
+      <c r="T3" t="n">
+        <v>1.048430553472623</v>
+      </c>
+      <c r="U3" t="n">
+        <v>1.036559103231528</v>
+      </c>
+      <c r="V3" t="n">
+        <v>1.021600796217383</v>
+      </c>
+      <c r="W3" t="n">
+        <v>1.003446662171047</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0.977675049242084</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0.9410503815130995</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>0.8848883407251702</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0.7878691540197655</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>0.5776967071458323</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>-0.1953417667144214</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>-4.730611029823361</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>-1.6435627200339</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>-1.291338759466204</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.920907218018398</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.9201489097169768</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.9193470426252427</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9184977526011414</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.9175967045198468</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.8904508009873416</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.8869280815641903</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.8829465524560606</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.8784103347291875</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.8731948343849674</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.8868867000131977</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.8828996036853635</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.8783566147655896</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.8731327653079377</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.8670625950140909</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.862536657544399</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.8545367950982093</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.8448860486614632</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.8330145984203675</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0.818056291406223</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0.7999021573598868</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0.7741305444309241</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0.7375058767019396</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0.6813438359140103</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0.5843246492086056</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>0.3741522023346724</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>-0.3988862715255813</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>-4.934155534634522</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>-1.84710722484506</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>-1.494883264277364</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.9585797923081611</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.9578214840067399</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.9570196169150058</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.9561703268909045</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.9552692788096099</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.9281233752771048</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.9246006558539535</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.9206191267458237</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.9160829090189506</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.9108674086747305</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.9245592743029608</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.9205721779751266</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.9160291890553527</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.9108053395977008</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.904735169303854</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.9002092318341621</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.8922093693879725</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.8825586229512263</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.8706871727101306</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.8557288656959862</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.8375747316496499</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0.8118031187206872</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0.7751784509917027</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.7190164102037734</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0.6219972234983687</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0.4118247766244355</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>-0.3612136972358182</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>-4.896482960344758</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>-1.809434650555297</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>-1.4572106899876</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.9264782493545758</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.9257199410531546</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.9249180739614205</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.9240687839373192</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.9231677358560245</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.8960218323235194</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.8924991129003681</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.8885175837922383</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.8839813660653653</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.8787658657211451</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.8924577313493754</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.8884706350215412</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.8839276461017673</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.8787037966441155</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.8726336263502686</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.8681076888805768</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.8601078264343871</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.850457079997641</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.8385856297565453</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.8236273227424008</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.8054731886960645</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.7797015757671019</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0.7430769080381173</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0.686914867250188</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0.5898956805447834</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0.3797232336708501</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>-0.3933152401894036</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>-4.928584503298344</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>-1.841536193508883</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>-1.489312232941186</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.9196770539162276</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.9189187456148064</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.9181168785230722</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.9172675884989709</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.9163665404176763</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.8892206368851712</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.8856979174620199</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.8817163883538901</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.877180170627017</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.8719646702827969</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.8856565359110272</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.881669439583193</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.8771264506634191</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.8719026012057672</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.8658324309119204</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.8613064934422285</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.8533066309960389</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.8436558845592927</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.831784434318197</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.8168261273040526</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.7986719932577163</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0.7729003803287536</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0.7362757125997691</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0.6801136718118398</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>0.5830944851064351</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>0.3729220382325019</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>-0.4001164356277518</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>-4.935385698736692</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>-1.848337388947231</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>-1.496113428379534</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1.015422745571573</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.014664437270151</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.013862570178417</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.013013280154316</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.012112232073021</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.9849663285405164</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.9814436091173651</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.9774620800092353</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.9729258622823622</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.9677103619381421</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.9814022275663724</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.9774151312385382</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.9728721423187643</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.9676482928611124</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.9615781225672656</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.9570521850975737</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.9490523226513841</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.9394015762146379</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.9275301259735422</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.9125718189593978</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.8944176849130615</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0.8686460719840988</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0.8320214042551143</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0.775859363467185</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>0.6788401767617803</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0.4686677298878471</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>-0.3043707439724066</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>-4.839640007081347</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>-1.752591697291886</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>-1.400367736724189</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.8856559237347353</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.8848976154333141</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.88409574834158</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.8832464583174787</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.8823454102361841</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.8551995067036789</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.8516767872805276</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.8476952581723979</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.8431590404455248</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.8379435401013047</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.851635405729535</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.8476483094017008</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.8431053204819269</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.837881471024275</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.8318113007304282</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.8272853632607363</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.8192855008145467</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.8096347543778005</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.7977633041367048</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.7828049971225604</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0.7646508630762241</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0.7388792501472614</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0.7022545824182769</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>0.6460925416303476</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>0.5490733549249429</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>0.3389009080510098</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>-0.434137565809244</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>-4.969406828918184</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>-1.882358519128723</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>-1.530134558561026</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.9841865146758176</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.9834282063743964</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.9826263392826623</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.981777049258561</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.9808760011772664</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.9537300976447612</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.9502073782216099</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.9462258491134802</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.9416896313866071</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.936474131042387</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.9501659966706173</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.9461789003427831</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.9416359114230092</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.9364120619653573</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.9303418916715105</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.9258159542018186</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.9178160917556289</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.9081653453188828</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0.8962938950777871</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.8813355880636426</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.8631814540173064</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0.8374098410883437</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0.8007851733593592</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0.7446231325714299</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>0.6476039458660252</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0.437431498992092</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>-0.3356069748681617</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>-4.870876237977102</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>-1.783827928187641</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>-1.431603967619944</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.065172225160831</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.06441391685941</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1.063612049767675</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1.062762759743574</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.061861711662279</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.034715808129774</v>
+      </c>
+      <c r="I11" t="n">
+        <v>1.031193088706623</v>
+      </c>
+      <c r="J11" t="n">
+        <v>1.027211559598493</v>
+      </c>
+      <c r="K11" t="n">
+        <v>1.02267534187162</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1.0174598415274</v>
+      </c>
+      <c r="M11" t="n">
+        <v>1.03115170715563</v>
+      </c>
+      <c r="N11" t="n">
+        <v>1.027164610827796</v>
+      </c>
+      <c r="O11" t="n">
+        <v>1.022621621908022</v>
+      </c>
+      <c r="P11" t="n">
+        <v>1.01739777245037</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>1.011327602156524</v>
+      </c>
+      <c r="R11" t="n">
+        <v>1.006801664686832</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.998801802240642</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.9891510558038958</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.9772796055628001</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.9623212985486558</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0.9441671645023195</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0.9183955515733568</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0.8817708838443723</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0.825608843056443</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>0.7285896563510383</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0.5184172094771051</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>-0.2546212643831486</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>-4.789890527492089</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>-1.702842217702628</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>-1.350618257134931</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -434,1058 +1499,1058 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="2" t="n">
         <v>2020</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="2" t="n">
         <v>2021</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="2" t="n">
         <v>2022</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="2" t="n">
         <v>2023</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="2" t="n">
         <v>2024</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="G1" s="2" t="n">
         <v>2025</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="H1" s="2" t="n">
         <v>2026</v>
       </c>
-      <c r="I1" s="1" t="n">
+      <c r="I1" s="2" t="n">
         <v>2027</v>
       </c>
-      <c r="J1" s="1" t="n">
+      <c r="J1" s="2" t="n">
         <v>2028</v>
       </c>
-      <c r="K1" s="1" t="n">
+      <c r="K1" s="2" t="n">
         <v>2029</v>
       </c>
-      <c r="L1" s="1" t="n">
+      <c r="L1" s="2" t="n">
         <v>2030</v>
       </c>
-      <c r="M1" s="1" t="n">
+      <c r="M1" s="2" t="n">
         <v>2031</v>
       </c>
-      <c r="N1" s="1" t="n">
+      <c r="N1" s="2" t="n">
         <v>2032</v>
       </c>
-      <c r="O1" s="1" t="n">
+      <c r="O1" s="2" t="n">
         <v>2033</v>
       </c>
-      <c r="P1" s="1" t="n">
+      <c r="P1" s="2" t="n">
         <v>2034</v>
       </c>
-      <c r="Q1" s="1" t="n">
+      <c r="Q1" s="2" t="n">
         <v>2035</v>
       </c>
-      <c r="R1" s="1" t="n">
+      <c r="R1" s="2" t="n">
         <v>2036</v>
       </c>
-      <c r="S1" s="1" t="n">
+      <c r="S1" s="2" t="n">
         <v>2037</v>
       </c>
-      <c r="T1" s="1" t="n">
+      <c r="T1" s="2" t="n">
         <v>2038</v>
       </c>
-      <c r="U1" s="1" t="n">
+      <c r="U1" s="2" t="n">
         <v>2039</v>
       </c>
-      <c r="V1" s="1" t="n">
+      <c r="V1" s="2" t="n">
         <v>2040</v>
       </c>
-      <c r="W1" s="1" t="n">
+      <c r="W1" s="2" t="n">
         <v>2041</v>
       </c>
-      <c r="X1" s="1" t="n">
+      <c r="X1" s="2" t="n">
         <v>2042</v>
       </c>
-      <c r="Y1" s="1" t="n">
+      <c r="Y1" s="2" t="n">
         <v>2043</v>
       </c>
-      <c r="Z1" s="1" t="n">
+      <c r="Z1" s="2" t="n">
         <v>2044</v>
       </c>
-      <c r="AA1" s="1" t="n">
+      <c r="AA1" s="2" t="n">
         <v>2045</v>
       </c>
-      <c r="AB1" s="1" t="n">
+      <c r="AB1" s="2" t="n">
         <v>2046</v>
       </c>
-      <c r="AC1" s="1" t="n">
+      <c r="AC1" s="2" t="n">
         <v>2047</v>
       </c>
-      <c r="AD1" s="1" t="n">
+      <c r="AD1" s="2" t="n">
         <v>2048</v>
       </c>
-      <c r="AE1" s="1" t="n">
+      <c r="AE1" s="2" t="n">
         <v>2049</v>
       </c>
-      <c r="AF1" s="1" t="n">
+      <c r="AF1" s="2" t="n">
         <v>2050</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
+      <c r="A2" s="2" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="n">
-        <v>0.9983027155686909</v>
+        <v>0.9397314474149884</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9975444072672697</v>
+        <v>0.9392011291978329</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9967425401755355</v>
+        <v>0.938645513804637</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9958932501514343</v>
+        <v>0.9380627469240425</v>
       </c>
       <c r="G2" t="n">
-        <v>0.9949922020701396</v>
+        <v>0.9374507884748424</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9678462985376345</v>
+        <v>0.9360058073087588</v>
       </c>
       <c r="I2" t="n">
-        <v>0.9643235791144832</v>
+        <v>0.9352849571664574</v>
       </c>
       <c r="J2" t="n">
-        <v>0.9603420500063534</v>
+        <v>0.9345237788105428</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9558058322794803</v>
+        <v>0.9337187905857558</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9505903319352602</v>
+        <v>0.9328660981861033</v>
       </c>
       <c r="M2" t="n">
-        <v>0.9642821975634905</v>
+        <v>0.9560879751718288</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9602951012356563</v>
+        <v>0.9560466416876775</v>
       </c>
       <c r="O2" t="n">
-        <v>0.9557521123158824</v>
+        <v>0.9560047715558289</v>
       </c>
       <c r="P2" t="n">
-        <v>0.9505282628582306</v>
+        <v>0.9559623542567548</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.9444580925643837</v>
+        <v>0.9559193789941753</v>
       </c>
       <c r="R2" t="n">
-        <v>0.9399321550946919</v>
+        <v>0.9606893277223642</v>
       </c>
       <c r="S2" t="n">
-        <v>0.9319322926485022</v>
+        <v>0.9606860561051769</v>
       </c>
       <c r="T2" t="n">
-        <v>0.9222815462117561</v>
+        <v>0.9606827726206481</v>
       </c>
       <c r="U2" t="n">
-        <v>0.9104100959706604</v>
+        <v>0.9606794772040895</v>
       </c>
       <c r="V2" t="n">
-        <v>0.8954517889565159</v>
+        <v>0.9606761697903423</v>
       </c>
       <c r="W2" t="n">
-        <v>0.8772976549101796</v>
+        <v>0.962561151635515</v>
       </c>
       <c r="X2" t="n">
-        <v>0.851526041981217</v>
+        <v>0.9625611474499867</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.8149013742522324</v>
+        <v>0.9625611432649999</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.7587393334643031</v>
+        <v>0.9625611390805546</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.6617201467588985</v>
+        <v>0.9625611348966505</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.4515476998849652</v>
+        <v>0.9632121901124877</v>
       </c>
       <c r="AC2" t="n">
-        <v>-0.3214907739752885</v>
+        <v>0.9632116782005322</v>
       </c>
       <c r="AD2" t="n">
-        <v>-4.856760037084229</v>
+        <v>0.9632111670203172</v>
       </c>
       <c r="AE2" t="n">
-        <v>-1.769711727294768</v>
+        <v>0.9632106565702745</v>
       </c>
       <c r="AF2" t="n">
-        <v>-1.417487766727071</v>
+        <v>0.9632101468488412</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="n">
-        <v>0.9555826385044416</v>
+        <v>0.922051229664257</v>
       </c>
       <c r="D3" t="n">
-        <v>0.9548243302030204</v>
+        <v>0.9215209114471016</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9540224631112862</v>
+        <v>0.9209652960539056</v>
       </c>
       <c r="F3" t="n">
-        <v>0.953173173087185</v>
+        <v>0.9203825291733111</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9522721250058903</v>
+        <v>0.9197705707241111</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9251262214733852</v>
+        <v>0.9183255895580275</v>
       </c>
       <c r="I3" t="n">
-        <v>0.9216035020502339</v>
+        <v>0.9176047394157261</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9176219729421041</v>
+        <v>0.9168435610598115</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9130857552152311</v>
+        <v>0.9160385728350244</v>
       </c>
       <c r="L3" t="n">
-        <v>0.9078702548710109</v>
+        <v>0.915185880435372</v>
       </c>
       <c r="M3" t="n">
-        <v>0.9215621204992412</v>
+        <v>0.9384077574210974</v>
       </c>
       <c r="N3" t="n">
-        <v>0.917575024171407</v>
+        <v>0.9383664239369461</v>
       </c>
       <c r="O3" t="n">
-        <v>0.9130320352516331</v>
+        <v>0.9383245538050975</v>
       </c>
       <c r="P3" t="n">
-        <v>0.9078081857939813</v>
+        <v>0.9382821365060234</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.9017380155001344</v>
+        <v>0.938239161243444</v>
       </c>
       <c r="R3" t="n">
-        <v>0.8972120780304426</v>
+        <v>0.9430091099716328</v>
       </c>
       <c r="S3" t="n">
-        <v>0.8892122155842529</v>
+        <v>0.9430058383544455</v>
       </c>
       <c r="T3" t="n">
-        <v>0.8795614691475068</v>
+        <v>0.9430025548699167</v>
       </c>
       <c r="U3" t="n">
-        <v>0.8676900189064111</v>
+        <v>0.9429992594533582</v>
       </c>
       <c r="V3" t="n">
-        <v>0.8527317118922666</v>
+        <v>0.942995952039611</v>
       </c>
       <c r="W3" t="n">
-        <v>0.8345775778459303</v>
+        <v>0.9448809338847837</v>
       </c>
       <c r="X3" t="n">
-        <v>0.8088059649169677</v>
+        <v>0.9448809296992553</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.7721812971879831</v>
+        <v>0.9448809255142685</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.7160192564000538</v>
+        <v>0.9448809213298233</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.6190000696946492</v>
+        <v>0.9448809171459192</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.408827622820716</v>
+        <v>0.9455319723617563</v>
       </c>
       <c r="AC3" t="n">
-        <v>-0.3642108510395377</v>
+        <v>0.9455314604498009</v>
       </c>
       <c r="AD3" t="n">
-        <v>-4.899480114148478</v>
+        <v>0.9455309492695858</v>
       </c>
       <c r="AE3" t="n">
-        <v>-1.812431804359017</v>
+        <v>0.9455304388195431</v>
       </c>
       <c r="AF3" t="n">
-        <v>-1.46020784379132</v>
+        <v>0.9455299290981098</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="n">
-        <v>0.9596781156805632</v>
+        <v>0.8907577123906656</v>
       </c>
       <c r="D4" t="n">
-        <v>0.9589198073791421</v>
+        <v>0.8902273941735102</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9581179402874078</v>
+        <v>0.8896717787803142</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9572686502633065</v>
+        <v>0.8890890118997197</v>
       </c>
       <c r="G4" t="n">
-        <v>0.956367602182012</v>
+        <v>0.8884770534505196</v>
       </c>
       <c r="H4" t="n">
-        <v>0.9292216986495068</v>
+        <v>0.887032072284436</v>
       </c>
       <c r="I4" t="n">
-        <v>0.9256989792263555</v>
+        <v>0.8863112221421346</v>
       </c>
       <c r="J4" t="n">
-        <v>0.9217174501182257</v>
+        <v>0.88555004378622</v>
       </c>
       <c r="K4" t="n">
-        <v>0.9171812323913526</v>
+        <v>0.884745055561433</v>
       </c>
       <c r="L4" t="n">
-        <v>0.9119657320471326</v>
+        <v>0.8838923631617805</v>
       </c>
       <c r="M4" t="n">
-        <v>0.9256575976753629</v>
+        <v>0.907114240147506</v>
       </c>
       <c r="N4" t="n">
-        <v>0.9216705013475286</v>
+        <v>0.9070729066633547</v>
       </c>
       <c r="O4" t="n">
-        <v>0.9171275124277547</v>
+        <v>0.9070310365315061</v>
       </c>
       <c r="P4" t="n">
-        <v>0.9119036629701029</v>
+        <v>0.906988619232432</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.9058334926762561</v>
+        <v>0.9069456439698526</v>
       </c>
       <c r="R4" t="n">
-        <v>0.9013075552065641</v>
+        <v>0.9117155926980414</v>
       </c>
       <c r="S4" t="n">
-        <v>0.8933076927603745</v>
+        <v>0.9117123210808541</v>
       </c>
       <c r="T4" t="n">
-        <v>0.8836569463236283</v>
+        <v>0.9117090375963253</v>
       </c>
       <c r="U4" t="n">
-        <v>0.8717854960825326</v>
+        <v>0.9117057421797667</v>
       </c>
       <c r="V4" t="n">
-        <v>0.8568271890683883</v>
+        <v>0.9117024347660195</v>
       </c>
       <c r="W4" t="n">
-        <v>0.838673055022052</v>
+        <v>0.9135874166111922</v>
       </c>
       <c r="X4" t="n">
-        <v>0.8129014420930893</v>
+        <v>0.9135874124256639</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.7762767743641048</v>
+        <v>0.9135874082406771</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.7201147335761755</v>
+        <v>0.9135874040562318</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.6230955468707708</v>
+        <v>0.9135873998723277</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.4129230999968376</v>
+        <v>0.9142384550881649</v>
       </c>
       <c r="AC4" t="n">
-        <v>-0.3601153738634161</v>
+        <v>0.9142379431762094</v>
       </c>
       <c r="AD4" t="n">
-        <v>-4.895384636972357</v>
+        <v>0.9142374319959944</v>
       </c>
       <c r="AE4" t="n">
-        <v>-1.808336327182895</v>
+        <v>0.9142369215459517</v>
       </c>
       <c r="AF4" t="n">
-        <v>-1.456112366615198</v>
+        <v>0.9142364118245184</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="n">
-        <v>1.095161147701316</v>
+        <v>1.140772176010125</v>
       </c>
       <c r="D5" t="n">
-        <v>1.094402839399894</v>
+        <v>1.14024185779297</v>
       </c>
       <c r="E5" t="n">
-        <v>1.09360097230816</v>
+        <v>1.139686242399774</v>
       </c>
       <c r="F5" t="n">
-        <v>1.092751682284059</v>
+        <v>1.139103475519179</v>
       </c>
       <c r="G5" t="n">
-        <v>1.091850634202764</v>
+        <v>1.138491517069979</v>
       </c>
       <c r="H5" t="n">
-        <v>1.064704730670259</v>
+        <v>1.137046535903895</v>
       </c>
       <c r="I5" t="n">
-        <v>1.061182011247108</v>
+        <v>1.136325685761594</v>
       </c>
       <c r="J5" t="n">
-        <v>1.057200482138978</v>
+        <v>1.135564507405679</v>
       </c>
       <c r="K5" t="n">
-        <v>1.052664264412105</v>
+        <v>1.134759519180893</v>
       </c>
       <c r="L5" t="n">
-        <v>1.047448764067885</v>
+        <v>1.13390682678124</v>
       </c>
       <c r="M5" t="n">
-        <v>1.061140629696115</v>
+        <v>1.157128703766966</v>
       </c>
       <c r="N5" t="n">
-        <v>1.057153533368281</v>
+        <v>1.157087370282814</v>
       </c>
       <c r="O5" t="n">
-        <v>1.052610544448507</v>
+        <v>1.157045500150966</v>
       </c>
       <c r="P5" t="n">
-        <v>1.047386694990855</v>
+        <v>1.157003082851892</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.041316524697008</v>
+        <v>1.156960107589312</v>
       </c>
       <c r="R5" t="n">
-        <v>1.036790587227316</v>
+        <v>1.161730056317501</v>
       </c>
       <c r="S5" t="n">
-        <v>1.028790724781127</v>
+        <v>1.161726784700314</v>
       </c>
       <c r="T5" t="n">
-        <v>1.019139978344381</v>
+        <v>1.161723501215785</v>
       </c>
       <c r="U5" t="n">
-        <v>1.007268528103285</v>
+        <v>1.161720205799226</v>
       </c>
       <c r="V5" t="n">
-        <v>0.9923102210891406</v>
+        <v>1.161716898385479</v>
       </c>
       <c r="W5" t="n">
-        <v>0.9741560870428043</v>
+        <v>1.163601880230652</v>
       </c>
       <c r="X5" t="n">
-        <v>0.9483844741138416</v>
+        <v>1.163601876045123</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.9117598063848571</v>
+        <v>1.163601871860137</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.8555977655969278</v>
+        <v>1.163601867675691</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.7585785788915231</v>
+        <v>1.163601863491787</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.5484061320175899</v>
+        <v>1.164252918707624</v>
       </c>
       <c r="AC5" t="n">
-        <v>-0.2246323418426638</v>
+        <v>1.164252406795669</v>
       </c>
       <c r="AD5" t="n">
-        <v>-4.759901604951605</v>
+        <v>1.164251895615454</v>
       </c>
       <c r="AE5" t="n">
-        <v>-1.672853295162143</v>
+        <v>1.164251385165411</v>
       </c>
       <c r="AF5" t="n">
-        <v>-1.320629334594446</v>
+        <v>1.164250875443978</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="n">
-        <v>0.9223288234291217</v>
+        <v>1.066451369283282</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9215705151277005</v>
+        <v>1.065921051066127</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9207686480359664</v>
+        <v>1.065365435672931</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9199193580118651</v>
+        <v>1.064782668792336</v>
       </c>
       <c r="G6" t="n">
-        <v>0.9190183099305704</v>
+        <v>1.064170710343136</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8918724063980653</v>
+        <v>1.062725729177052</v>
       </c>
       <c r="I6" t="n">
-        <v>0.888349686974914</v>
+        <v>1.062004879034751</v>
       </c>
       <c r="J6" t="n">
-        <v>0.8843681578667842</v>
+        <v>1.061243700678836</v>
       </c>
       <c r="K6" t="n">
-        <v>0.8798319401399112</v>
+        <v>1.060438712454049</v>
       </c>
       <c r="L6" t="n">
-        <v>0.874616439795691</v>
+        <v>1.059586020054397</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8883083054239214</v>
+        <v>1.082807897040122</v>
       </c>
       <c r="N6" t="n">
-        <v>0.8843212090960871</v>
+        <v>1.082766563555971</v>
       </c>
       <c r="O6" t="n">
-        <v>0.8797782201763132</v>
+        <v>1.082724693424122</v>
       </c>
       <c r="P6" t="n">
-        <v>0.8745543707186614</v>
+        <v>1.082682276125048</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.8684842004248146</v>
+        <v>1.082639300862469</v>
       </c>
       <c r="R6" t="n">
-        <v>0.8639582629551227</v>
+        <v>1.087409249590658</v>
       </c>
       <c r="S6" t="n">
-        <v>0.855958400508933</v>
+        <v>1.08740597797347</v>
       </c>
       <c r="T6" t="n">
-        <v>0.8463076540721869</v>
+        <v>1.087402694488942</v>
       </c>
       <c r="U6" t="n">
-        <v>0.8344362038310912</v>
+        <v>1.087399399072383</v>
       </c>
       <c r="V6" t="n">
-        <v>0.8194778968169467</v>
+        <v>1.087396091658636</v>
       </c>
       <c r="W6" t="n">
-        <v>0.8013237627706105</v>
+        <v>1.089281073503809</v>
       </c>
       <c r="X6" t="n">
-        <v>0.7755521498416478</v>
+        <v>1.08928106931828</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.7389274821126632</v>
+        <v>1.089281065133293</v>
       </c>
       <c r="Z6" t="n">
-        <v>0.6827654413247339</v>
+        <v>1.089281060948848</v>
       </c>
       <c r="AA6" t="n">
-        <v>0.5857462546193293</v>
+        <v>1.089281056764944</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.3755738077453961</v>
+        <v>1.089932111980781</v>
       </c>
       <c r="AC6" t="n">
-        <v>-0.3974646661148576</v>
+        <v>1.089931600068826</v>
       </c>
       <c r="AD6" t="n">
-        <v>-4.932733929223798</v>
+        <v>1.089931088888611</v>
       </c>
       <c r="AE6" t="n">
-        <v>-1.845685619434337</v>
+        <v>1.089930578438568</v>
       </c>
       <c r="AF6" t="n">
-        <v>-1.49346165886664</v>
+        <v>1.089930068717135</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="2" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="n">
-        <v>0.9767056701777337</v>
+        <v>0.9604469357602434</v>
       </c>
       <c r="D7" t="n">
-        <v>0.9759473618763125</v>
+        <v>0.959916617543088</v>
       </c>
       <c r="E7" t="n">
-        <v>0.9751454947845783</v>
+        <v>0.9593610021498922</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9742962047604771</v>
+        <v>0.9587782352692975</v>
       </c>
       <c r="G7" t="n">
-        <v>0.9733951566791824</v>
+        <v>0.9581662768200976</v>
       </c>
       <c r="H7" t="n">
-        <v>0.9462492531466773</v>
+        <v>0.9567212956540139</v>
       </c>
       <c r="I7" t="n">
-        <v>0.942726533723526</v>
+        <v>0.9560004455117126</v>
       </c>
       <c r="J7" t="n">
-        <v>0.9387450046153962</v>
+        <v>0.9552392671557979</v>
       </c>
       <c r="K7" t="n">
-        <v>0.9342087868885232</v>
+        <v>0.954434278931011</v>
       </c>
       <c r="L7" t="n">
-        <v>0.928993286544303</v>
+        <v>0.9535815865313584</v>
       </c>
       <c r="M7" t="n">
-        <v>0.9426851521725333</v>
+        <v>0.9768034635170839</v>
       </c>
       <c r="N7" t="n">
-        <v>0.9386980558446991</v>
+        <v>0.9767621300329326</v>
       </c>
       <c r="O7" t="n">
-        <v>0.9341550669249252</v>
+        <v>0.976720259901084</v>
       </c>
       <c r="P7" t="n">
-        <v>0.9289312174672734</v>
+        <v>0.97667784260201</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.9228610471734265</v>
+        <v>0.9766348673394305</v>
       </c>
       <c r="R7" t="n">
-        <v>0.9183351097037347</v>
+        <v>0.9814048160676192</v>
       </c>
       <c r="S7" t="n">
-        <v>0.910335247257545</v>
+        <v>0.981401544450432</v>
       </c>
       <c r="T7" t="n">
-        <v>0.9006845008207989</v>
+        <v>0.9813982609659031</v>
       </c>
       <c r="U7" t="n">
-        <v>0.8888130505797032</v>
+        <v>0.9813949655493446</v>
       </c>
       <c r="V7" t="n">
-        <v>0.8738547435655587</v>
+        <v>0.9813916581355975</v>
       </c>
       <c r="W7" t="n">
-        <v>0.8557006095192224</v>
+        <v>0.9832766399807702</v>
       </c>
       <c r="X7" t="n">
-        <v>0.8299289965902598</v>
+        <v>0.9832766357952418</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.7933043288612752</v>
+        <v>0.983276631610255</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.7371422880733459</v>
+        <v>0.9832766274258098</v>
       </c>
       <c r="AA7" t="n">
-        <v>0.6401231013679413</v>
+        <v>0.9832766232419057</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.429950654494008</v>
+        <v>0.9839276784577429</v>
       </c>
       <c r="AC7" t="n">
-        <v>-0.3430878193662457</v>
+        <v>0.9839271665457874</v>
       </c>
       <c r="AD7" t="n">
-        <v>-4.878357082475186</v>
+        <v>0.9839266553655723</v>
       </c>
       <c r="AE7" t="n">
-        <v>-1.791308772685725</v>
+        <v>0.9839261449155297</v>
       </c>
       <c r="AF7" t="n">
-        <v>-1.439084812118028</v>
+        <v>0.9839256351940964</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="2" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="n">
-        <v>0.8965646696254003</v>
+        <v>0.9093950089785153</v>
       </c>
       <c r="D8" t="n">
-        <v>0.8958063613239791</v>
+        <v>0.9088646907613599</v>
       </c>
       <c r="E8" t="n">
-        <v>0.8950044942322449</v>
+        <v>0.908309075368164</v>
       </c>
       <c r="F8" t="n">
-        <v>0.8941552042081437</v>
+        <v>0.9077263084875694</v>
       </c>
       <c r="G8" t="n">
-        <v>0.893254156126849</v>
+        <v>0.9071143500383694</v>
       </c>
       <c r="H8" t="n">
-        <v>0.8661082525943439</v>
+        <v>0.9056693688722858</v>
       </c>
       <c r="I8" t="n">
-        <v>0.8625855331711926</v>
+        <v>0.9049485187299844</v>
       </c>
       <c r="J8" t="n">
-        <v>0.8586040040630628</v>
+        <v>0.9041873403740698</v>
       </c>
       <c r="K8" t="n">
-        <v>0.8540677863361897</v>
+        <v>0.9033823521492828</v>
       </c>
       <c r="L8" t="n">
-        <v>0.8488522859919696</v>
+        <v>0.9025296597496303</v>
       </c>
       <c r="M8" t="n">
-        <v>0.8625441516201999</v>
+        <v>0.9257515367353557</v>
       </c>
       <c r="N8" t="n">
-        <v>0.8585570552923657</v>
+        <v>0.9257102032512045</v>
       </c>
       <c r="O8" t="n">
-        <v>0.8540140663725918</v>
+        <v>0.9256683331193558</v>
       </c>
       <c r="P8" t="n">
-        <v>0.8487902169149399</v>
+        <v>0.9256259158202818</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.8427200466210931</v>
+        <v>0.9255829405577023</v>
       </c>
       <c r="R8" t="n">
-        <v>0.8381941091514012</v>
+        <v>0.9303528892858911</v>
       </c>
       <c r="S8" t="n">
-        <v>0.8301942467052116</v>
+        <v>0.9303496176687038</v>
       </c>
       <c r="T8" t="n">
-        <v>0.8205435002684655</v>
+        <v>0.930346334184175</v>
       </c>
       <c r="U8" t="n">
-        <v>0.8086720500273697</v>
+        <v>0.9303430387676165</v>
       </c>
       <c r="V8" t="n">
-        <v>0.7937137430132253</v>
+        <v>0.9303397313538693</v>
       </c>
       <c r="W8" t="n">
-        <v>0.775559608966889</v>
+        <v>0.932224713199042</v>
       </c>
       <c r="X8" t="n">
-        <v>0.7497879960379263</v>
+        <v>0.9322247090135136</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.7131633283089418</v>
+        <v>0.9322247048285268</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.6570012875210125</v>
+        <v>0.9322247006440816</v>
       </c>
       <c r="AA8" t="n">
-        <v>0.5599821008156078</v>
+        <v>0.9322246964601775</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.3498096539416746</v>
+        <v>0.9328757516760147</v>
       </c>
       <c r="AC8" t="n">
-        <v>-0.4232288199185791</v>
+        <v>0.9328752397640592</v>
       </c>
       <c r="AD8" t="n">
-        <v>-4.95849808302752</v>
+        <v>0.9328747285838441</v>
       </c>
       <c r="AE8" t="n">
-        <v>-1.871449773238058</v>
+        <v>0.9328742181338014</v>
       </c>
       <c r="AF8" t="n">
-        <v>-1.519225812670361</v>
+        <v>0.9328737084123682</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="2" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="n">
-        <v>0.9595701115408425</v>
+        <v>0.9703994102015514</v>
       </c>
       <c r="D9" t="n">
-        <v>0.9588118032394213</v>
+        <v>0.969869091984396</v>
       </c>
       <c r="E9" t="n">
-        <v>0.9580099361476871</v>
+        <v>0.9693134765912</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9571606461235859</v>
+        <v>0.9687307097106055</v>
       </c>
       <c r="G9" t="n">
-        <v>0.9562595980422912</v>
+        <v>0.9681187512614055</v>
       </c>
       <c r="H9" t="n">
-        <v>0.9291136945097861</v>
+        <v>0.9666737700953218</v>
       </c>
       <c r="I9" t="n">
-        <v>0.9255909750866348</v>
+        <v>0.9659529199530205</v>
       </c>
       <c r="J9" t="n">
-        <v>0.921609445978505</v>
+        <v>0.9651917415971059</v>
       </c>
       <c r="K9" t="n">
-        <v>0.917073228251632</v>
+        <v>0.9643867533723188</v>
       </c>
       <c r="L9" t="n">
-        <v>0.9118577279074118</v>
+        <v>0.9635340609726664</v>
       </c>
       <c r="M9" t="n">
-        <v>0.9255495935356421</v>
+        <v>0.9867559379583918</v>
       </c>
       <c r="N9" t="n">
-        <v>0.9215624972078079</v>
+        <v>0.9867146044742405</v>
       </c>
       <c r="O9" t="n">
-        <v>0.917019508288034</v>
+        <v>0.9866727343423919</v>
       </c>
       <c r="P9" t="n">
-        <v>0.9117956588303822</v>
+        <v>0.9866303170433178</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.9057254885365353</v>
+        <v>0.9865873417807384</v>
       </c>
       <c r="R9" t="n">
-        <v>0.9011995510668435</v>
+        <v>0.9913572905089272</v>
       </c>
       <c r="S9" t="n">
-        <v>0.8931996886206538</v>
+        <v>0.9913540188917399</v>
       </c>
       <c r="T9" t="n">
-        <v>0.8835489421839077</v>
+        <v>0.9913507354072111</v>
       </c>
       <c r="U9" t="n">
-        <v>0.871677491942812</v>
+        <v>0.9913474399906526</v>
       </c>
       <c r="V9" t="n">
-        <v>0.8567191849286675</v>
+        <v>0.9913441325769053</v>
       </c>
       <c r="W9" t="n">
-        <v>0.8385650508823312</v>
+        <v>0.9932291144220781</v>
       </c>
       <c r="X9" t="n">
-        <v>0.8127934379533686</v>
+        <v>0.9932291102365497</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.776168770224384</v>
+        <v>0.9932291060515629</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.7200067294364547</v>
+        <v>0.9932291018671177</v>
       </c>
       <c r="AA9" t="n">
-        <v>0.6229875427310501</v>
+        <v>0.9932290976832135</v>
       </c>
       <c r="AB9" t="n">
-        <v>0.4128150958571168</v>
+        <v>0.9938801528990507</v>
       </c>
       <c r="AC9" t="n">
-        <v>-0.3602233780031369</v>
+        <v>0.9938796409870952</v>
       </c>
       <c r="AD9" t="n">
-        <v>-4.895492641112077</v>
+        <v>0.9938791298068802</v>
       </c>
       <c r="AE9" t="n">
-        <v>-1.808444331322616</v>
+        <v>0.9938786193568375</v>
       </c>
       <c r="AF9" t="n">
-        <v>-1.456220370754919</v>
+        <v>0.9938781096354042</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="2" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="n">
-        <v>1.01731163995365</v>
+        <v>1.080824882125417</v>
       </c>
       <c r="D10" t="n">
-        <v>1.016553331652229</v>
+        <v>1.080294563908262</v>
       </c>
       <c r="E10" t="n">
-        <v>1.015751464560495</v>
+        <v>1.079738948515065</v>
       </c>
       <c r="F10" t="n">
-        <v>1.014902174536393</v>
+        <v>1.079156181634471</v>
       </c>
       <c r="G10" t="n">
-        <v>1.014001126455099</v>
+        <v>1.078544223185271</v>
       </c>
       <c r="H10" t="n">
-        <v>0.9868552229225935</v>
+        <v>1.077099242019187</v>
       </c>
       <c r="I10" t="n">
-        <v>0.9833325034994422</v>
+        <v>1.076378391876886</v>
       </c>
       <c r="J10" t="n">
-        <v>0.9793509743913125</v>
+        <v>1.075617213520971</v>
       </c>
       <c r="K10" t="n">
-        <v>0.9748147566644394</v>
+        <v>1.074812225296184</v>
       </c>
       <c r="L10" t="n">
-        <v>0.9695992563202191</v>
+        <v>1.073959532896532</v>
       </c>
       <c r="M10" t="n">
-        <v>0.9832911219484495</v>
+        <v>1.097181409882257</v>
       </c>
       <c r="N10" t="n">
-        <v>0.9793040256206154</v>
+        <v>1.097140076398106</v>
       </c>
       <c r="O10" t="n">
-        <v>0.9747610367008415</v>
+        <v>1.097098206266257</v>
       </c>
       <c r="P10" t="n">
-        <v>0.9695371872431895</v>
+        <v>1.097055788967183</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.9634670169493427</v>
+        <v>1.097012813704604</v>
       </c>
       <c r="R10" t="n">
-        <v>0.9589410794796509</v>
+        <v>1.101782762432793</v>
       </c>
       <c r="S10" t="n">
-        <v>0.9509412170334612</v>
+        <v>1.101779490815605</v>
       </c>
       <c r="T10" t="n">
-        <v>0.9412904705967151</v>
+        <v>1.101776207331077</v>
       </c>
       <c r="U10" t="n">
-        <v>0.9294190203556194</v>
+        <v>1.101772911914518</v>
       </c>
       <c r="V10" t="n">
-        <v>0.9144607133414748</v>
+        <v>1.101769604500771</v>
       </c>
       <c r="W10" t="n">
-        <v>0.8963065792951386</v>
+        <v>1.103654586345943</v>
       </c>
       <c r="X10" t="n">
-        <v>0.8705349663661759</v>
+        <v>1.103654582160415</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.8339102986371913</v>
+        <v>1.103654577975428</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.777748257849262</v>
+        <v>1.103654573790983</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.6807290711438574</v>
+        <v>1.103654569607079</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.4705566242699242</v>
+        <v>1.104305624822916</v>
       </c>
       <c r="AC10" t="n">
-        <v>-0.3024818495903295</v>
+        <v>1.104305112910961</v>
       </c>
       <c r="AD10" t="n">
-        <v>-4.837751112699269</v>
+        <v>1.104304601730746</v>
       </c>
       <c r="AE10" t="n">
-        <v>-1.750702802909809</v>
+        <v>1.104304091280703</v>
       </c>
       <c r="AF10" t="n">
-        <v>-1.398478842342112</v>
+        <v>1.10430358155927</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="2" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="n">
-        <v>0.9471859259392015</v>
+        <v>0.8915197634857951</v>
       </c>
       <c r="D11" t="n">
-        <v>0.9464276176377803</v>
+        <v>0.8909894452686397</v>
       </c>
       <c r="E11" t="n">
-        <v>0.9456257505460461</v>
+        <v>0.8904338298754437</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9447764605219449</v>
+        <v>0.8898510629948492</v>
       </c>
       <c r="G11" t="n">
-        <v>0.9438754124406502</v>
+        <v>0.8892391045456491</v>
       </c>
       <c r="H11" t="n">
-        <v>0.9167295089081451</v>
+        <v>0.8877941233795655</v>
       </c>
       <c r="I11" t="n">
-        <v>0.9132067894849938</v>
+        <v>0.8870732732372641</v>
       </c>
       <c r="J11" t="n">
-        <v>0.909225260376864</v>
+        <v>0.8863120948813495</v>
       </c>
       <c r="K11" t="n">
-        <v>0.9046890426499909</v>
+        <v>0.8855071066565625</v>
       </c>
       <c r="L11" t="n">
-        <v>0.8994735423057708</v>
+        <v>0.88465441425691</v>
       </c>
       <c r="M11" t="n">
-        <v>0.9131654079340011</v>
+        <v>0.9078762912426355</v>
       </c>
       <c r="N11" t="n">
-        <v>0.9091783116061669</v>
+        <v>0.9078349577584842</v>
       </c>
       <c r="O11" t="n">
-        <v>0.904635322686393</v>
+        <v>0.9077930876266356</v>
       </c>
       <c r="P11" t="n">
-        <v>0.8994114732287412</v>
+        <v>0.9077506703275615</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.8933413029348943</v>
+        <v>0.9077076950649821</v>
       </c>
       <c r="R11" t="n">
-        <v>0.8888153654652025</v>
+        <v>0.9124776437931709</v>
       </c>
       <c r="S11" t="n">
-        <v>0.8808155030190128</v>
+        <v>0.9124743721759836</v>
       </c>
       <c r="T11" t="n">
-        <v>0.8711647565822667</v>
+        <v>0.9124710886914548</v>
       </c>
       <c r="U11" t="n">
-        <v>0.859293306341171</v>
+        <v>0.9124677932748962</v>
       </c>
       <c r="V11" t="n">
-        <v>0.8443349993270265</v>
+        <v>0.912464485861149</v>
       </c>
       <c r="W11" t="n">
-        <v>0.8261808652806902</v>
+        <v>0.9143494677063218</v>
       </c>
       <c r="X11" t="n">
-        <v>0.8004092523517276</v>
+        <v>0.9143494635207934</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.763784584622743</v>
+        <v>0.9143494593358066</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.7076225438348137</v>
+        <v>0.9143494551513613</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.6106033571294091</v>
+        <v>0.9143494509674572</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.4004309102554758</v>
+        <v>0.9150005061832944</v>
       </c>
       <c r="AC11" t="n">
-        <v>-0.3726075636047779</v>
+        <v>0.9149999942713389</v>
       </c>
       <c r="AD11" t="n">
-        <v>-4.907876826713718</v>
+        <v>0.9149994830911239</v>
       </c>
       <c r="AE11" t="n">
-        <v>-1.820828516924257</v>
+        <v>0.9149989726410812</v>
       </c>
       <c r="AF11" t="n">
-        <v>-1.46860455635656</v>
+        <v>0.9149984629196479</v>
       </c>
     </row>
   </sheetData>

</xml_diff>